<commit_message>
FILE PROCESSING AND GRADE UPDATING MOSTLY DONE
# TODO:
1. Fix str comparing to float - Due to an issue in spreadsheets of either "EX" or whitespace probably
2. Use fuzzy matching for non-conventional student names
</commit_message>
<xml_diff>
--- a/Multiple-Assignments-(11-27-24).xlsx
+++ b/Multiple-Assignments-(11-27-24).xlsx
@@ -576,7 +576,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -588,13 +588,6 @@
       <sz val="11"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -1044,28 +1037,31 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1074,118 +1070,115 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1594,7 +1587,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1:C1"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1775,10 +1768,10 @@
         <v>0</v>
       </c>
       <c r="E4" s="2">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="F4" s="2">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="G4" s="2">
         <v>100</v>
@@ -1793,7 +1786,7 @@
         <v>100</v>
       </c>
       <c r="K4" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="L4" s="2">
         <v>90</v>
@@ -1826,7 +1819,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="F5" s="2">
         <v>55</v>
@@ -5715,11 +5708,11 @@
       </c>
       <c r="E83" s="5">
         <f t="shared" si="0"/>
-        <v>29.56</v>
+        <v>31.33</v>
       </c>
       <c r="F83" s="5">
         <f t="shared" si="0"/>
-        <v>41.96</v>
+        <v>42.15</v>
       </c>
       <c r="G83" s="5">
         <f t="shared" si="0"/>
@@ -5739,7 +5732,7 @@
       </c>
       <c r="K83" s="5">
         <f t="shared" si="0"/>
-        <v>43.97</v>
+        <v>44.61</v>
       </c>
       <c r="L83" s="5">
         <f t="shared" si="0"/>
@@ -5772,11 +5765,11 @@
       </c>
       <c r="E85" s="5">
         <f t="shared" si="1"/>
-        <v>33.04</v>
+        <v>38.04</v>
       </c>
       <c r="F85" s="5">
         <f t="shared" si="1"/>
-        <v>38.75</v>
+        <v>39.29</v>
       </c>
       <c r="G85" s="5">
         <f t="shared" si="1"/>
@@ -5796,7 +5789,7 @@
       </c>
       <c r="K85" s="5">
         <f t="shared" si="1"/>
-        <v>44.04</v>
+        <v>45.82</v>
       </c>
       <c r="L85" s="5">
         <f t="shared" si="1"/>

</xml_diff>